<commit_message>
list-medseventchanges-1 profile - corrected change-description extension
Referenced the correct URL and tidied up the associated definition.

CIFMM-2311
</commit_message>
<xml_diff>
--- a/output/EventSummary/list-medseventchanges-1.xlsx
+++ b/output/EventSummary/list-medseventchanges-1.xlsx
@@ -817,15 +817,14 @@
     <t>changeDescription</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/encounter-description]]} {[]}
+    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/change-description]]} {[]}
 </t>
   </si>
   <si>
-    <t>Description, overview or summary of an encounter</t>
-  </si>
-  <si>
-    <t>Description of the change to the medicine item
-URL: http://hl7.org.au/fhir/StructureDefinition/change-description</t>
+    <t>Change description</t>
+  </si>
+  <si>
+    <t>Description of the change to the medicine item</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}

</xml_diff>

<commit_message>
add examples tab to ES profile pages; fix extensions and examples table width in SHS
</commit_message>
<xml_diff>
--- a/output/EventSummary/list-medseventchanges-1.xlsx
+++ b/output/EventSummary/list-medseventchanges-1.xlsx
@@ -301,7 +301,7 @@
     <t>Profiles this resource claims to conform to</t>
   </si>
   <si>
-    <t>A list of profiles (references to [StructureDefinition](structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url]().</t>
+    <t>A list of profiles (references to [StructureDefinition](https://build.fhir.org/ig/hl7au/au-fhir-base/structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url](https://build.fhir.org/ig/hl7au/au-fhir-base/).</t>
   </si>
   <si>
     <t>It is up to the server and/or other infrastructure of policy to determine whether/how these claims are verified and/or updated over time.  The list of profile URLs is a set.</t>
@@ -2837,7 +2837,7 @@
         <v>39</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>41</v>

</xml_diff>

<commit_message>
ES output after merge
</commit_message>
<xml_diff>
--- a/output/EventSummary/list-medseventchanges-1.xlsx
+++ b/output/EventSummary/list-medseventchanges-1.xlsx
@@ -4712,7 +4712,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
         <v>262</v>
       </c>
@@ -4722,13 +4722,13 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F35" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>41</v>

</xml_diff>

<commit_message>
Regenerate ES outputs following PR acceptance
</commit_message>
<xml_diff>
--- a/output/EventSummary/list-medseventchanges-1.xlsx
+++ b/output/EventSummary/list-medseventchanges-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$32</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="259">
   <si>
     <t>Path</t>
   </si>
@@ -201,389 +201,257 @@
     <t>Resource.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-dh-lst-01:One meta.profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/list-medseventchanges-1' {meta.profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/list-medseventchanges-1').exists()}
+    <t>List.implicitRules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri {[]} {[]}
 </t>
   </si>
   <si>
-    <t>List.meta.id</t>
+    <t>A set of rules under which this content was created</t>
+  </si>
+  <si>
+    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content.</t>
+  </si>
+  <si>
+    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. 
+This element is labelled as a modifier because the implicit rules may provide additional knowledge about the resource that modifies it's meaning or interpretation.</t>
+  </si>
+  <si>
+    <t>Resource.implicitRules</t>
+  </si>
+  <si>
+    <t>List.language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Language of the resource content</t>
+  </si>
+  <si>
+    <t>The base language in which the resource is written.</t>
+  </si>
+  <si>
+    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource  Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>A human language.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/languages</t>
+  </si>
+  <si>
+    <t>Resource.language</t>
+  </si>
+  <si>
+    <t>List.text</t>
+  </si>
+  <si>
+    <t>narrative
+htmlxhtmldisplay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narrative {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Text summary of the resource, for human interpretation</t>
+  </si>
+  <si>
+    <t>A human-readable narrative that contains a summary of the resource, and may be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
+  </si>
+  <si>
+    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded in formation is added later.</t>
+  </si>
+  <si>
+    <t>DomainResource.text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dom-1
+</t>
+  </si>
+  <si>
+    <t>Act.text?</t>
+  </si>
+  <si>
+    <t>List.contained</t>
+  </si>
+  <si>
+    <t>inline resources
+anonymous resourcescontained resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Contained, inline Resources</t>
+  </si>
+  <si>
+    <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
+  </si>
+  <si>
+    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again.</t>
+  </si>
+  <si>
+    <t>DomainResource.contained</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>List.extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>sourceRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/list-source-role]]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Practitioner role that defined the list contents (aka Author)</t>
+  </si>
+  <si>
+    <t>The entity (practitioner role) responsible for deciding what the contents of the list were. Where the list was created by a human, this is the same as the author of the list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>List.modifierExtension</t>
+  </si>
+  <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
+    <t>Extensions that cannot be ignored</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
+    <t>DomainResource.modifierExtension</t>
+  </si>
+  <si>
+    <t>List.identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Business identifier</t>
+  </si>
+  <si>
+    <t>Identifier for the List assigned for business purposes outside the context of FHIR.</t>
+  </si>
+  <si>
+    <t>.id</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>List.status</t>
+  </si>
+  <si>
+    <t>current | retired | entered-in-error</t>
+  </si>
+  <si>
+    <t>Indicates the current state of this list.</t>
+  </si>
+  <si>
+    <t>This element is labeled as a modifier because the status contains codes that mark the resource as not currently valid.</t>
+  </si>
+  <si>
+    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="current"/&gt;</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>The current state of the list</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/list-status</t>
+  </si>
+  <si>
+    <t>.status[current=active;retired=obsolete;entered-in-error=nullified]</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>List.mode</t>
+  </si>
+  <si>
+    <t>working | snapshot | changes</t>
+  </si>
+  <si>
+    <t>How this list was prepared - whether it is a working list that is suitable for being maintained on an ongoing basis, or if it represents a snapshot of a list of items from another source, or whether it is a prepared list where items may be marked as added, modified or deleted.</t>
+  </si>
+  <si>
+    <t>This element is labeled as a modifier because a change list must not be mis-understood as a complete list.</t>
+  </si>
+  <si>
+    <t>Lists are used in various ways, and it must be known in what way it is safe to use them.</t>
+  </si>
+  <si>
+    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="snapshot"/&gt;</t>
+  </si>
+  <si>
+    <t>The processing mode that applies to this list</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/list-mode</t>
+  </si>
+  <si>
+    <t>.outBoundRelationship[typeCode=COMP].target[classCode=OBS"].value</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>List.title</t>
   </si>
   <si>
     <t xml:space="preserve">string {[]} {[]}
 </t>
-  </si>
-  <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>List.meta.extension</t>
-  </si>
-  <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Additional Content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>List.meta.versionId</t>
-  </si>
-  <si>
-    <t>Version specific identifier</t>
-  </si>
-  <si>
-    <t>The version specific identifier, as it appears in the version portion of the URL. This values changes when the resource is created, updated, or deleted.</t>
-  </si>
-  <si>
-    <t>The server assigns this value, and ignores what the client specifies, except in the case that the server is imposing version integrity on updates/deletes.</t>
-  </si>
-  <si>
-    <t>Meta.versionId</t>
-  </si>
-  <si>
-    <t>List.meta.lastUpdated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instant {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>When the resource version last changed</t>
-  </si>
-  <si>
-    <t>When the resource last changed - e.g. when the version changed.</t>
-  </si>
-  <si>
-    <t>This value is always populated except when the resource is first being created. The server / resource manager sets this value; what a client provides is irrelevant.</t>
-  </si>
-  <si>
-    <t>Meta.lastUpdated</t>
-  </si>
-  <si>
-    <t>List.meta.profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uri {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Profiles this resource claims to conform to</t>
-  </si>
-  <si>
-    <t>A list of profiles (references to [StructureDefinition](https://build.fhir.org/ig/hl7au/au-fhir-base/structuredefinition.html#) resources) that this resource claims to conform to. The URL is a reference to [StructureDefinition.url](https://build.fhir.org/ig/hl7au/au-fhir-base/).</t>
-  </si>
-  <si>
-    <t>It is up to the server and/or other infrastructure of policy to determine whether/how these claims are verified and/or updated over time.  The list of profile URLs is a set.</t>
-  </si>
-  <si>
-    <t>Meta.profile</t>
-  </si>
-  <si>
-    <t>List.meta.security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Security Labels applied to this resource</t>
-  </si>
-  <si>
-    <t>Security labels applied to this resource. These tags connect specific resources to the overall security policy and infrastructure.</t>
-  </si>
-  <si>
-    <t>The security labels can be updated without changing the stated version of the resource  The list of security labels is a set. Uniqueness is based the system/code, and version and display are ignored.</t>
-  </si>
-  <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>Security Labels from the Healthcare Privacy and Security Classification System.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/security-labels</t>
-  </si>
-  <si>
-    <t>Meta.security</t>
-  </si>
-  <si>
-    <t>List.meta.tag</t>
-  </si>
-  <si>
-    <t>Tags applied to this resource</t>
-  </si>
-  <si>
-    <t>Tags applied to this resource. Tags are intended to be used to identify and relate resources to process and workflow, and applications are not required to consider the tags when interpreting the meaning of a resource.</t>
-  </si>
-  <si>
-    <t>The tags can be updated without changing the stated version of the resource.  The list of tags is a set. Uniqueness is based the system/code, and version and display are ignored.</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Codes that represent various types of tags, commonly workflow-related; e.g. "Needs review by Dr. Jones"</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/common-tags</t>
-  </si>
-  <si>
-    <t>Meta.tag</t>
-  </si>
-  <si>
-    <t>List.implicitRules</t>
-  </si>
-  <si>
-    <t>A set of rules under which this content was created</t>
-  </si>
-  <si>
-    <t>A reference to a set of rules that were followed when the resource was constructed, and which must be understood when processing the content.</t>
-  </si>
-  <si>
-    <t>Asserting this rule set restricts the content to be only understood by a limited set of trading partners. This inherently limits the usefulness of the data in the long term. However, the existing health eco-system is highly fractured, and not yet ready to define, collect, and exchange data in a generally computable sense. Wherever possible, implementers and/or specification writers should avoid using this element. 
-This element is labelled as a modifier because the implicit rules may provide additional knowledge about the resource that modifies it's meaning or interpretation.</t>
-  </si>
-  <si>
-    <t>Resource.implicitRules</t>
-  </si>
-  <si>
-    <t>List.language</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Language of the resource content</t>
-  </si>
-  <si>
-    <t>The base language in which the resource is written.</t>
-  </si>
-  <si>
-    <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource  Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
-  </si>
-  <si>
-    <t>A human language.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
-  </si>
-  <si>
-    <t>Resource.language</t>
-  </si>
-  <si>
-    <t>List.text</t>
-  </si>
-  <si>
-    <t>narrative
-htmlxhtmldisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narrative {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Text summary of the resource, for human interpretation</t>
-  </si>
-  <si>
-    <t>A human-readable narrative that contains a summary of the resource, and may be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
-  </si>
-  <si>
-    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded in formation is added later.</t>
-  </si>
-  <si>
-    <t>DomainResource.text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dom-1
-</t>
-  </si>
-  <si>
-    <t>Act.text?</t>
-  </si>
-  <si>
-    <t>List.contained</t>
-  </si>
-  <si>
-    <t>inline resources
-anonymous resourcescontained resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resource {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Contained, inline Resources</t>
-  </si>
-  <si>
-    <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
-  </si>
-  <si>
-    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again.</t>
-  </si>
-  <si>
-    <t>DomainResource.contained</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>List.extension</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>sourceRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/list-source-role]]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Practitioner role that defined the list contents (aka Author)</t>
-  </si>
-  <si>
-    <t>The entity (practitioner role) responsible for deciding what the contents of the list were. Where the list was created by a human, this is the same as the author of the list.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>List.modifierExtension</t>
-  </si>
-  <si>
-    <t>Extensions that cannot be ignored</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
-  </si>
-  <si>
-    <t>DomainResource.modifierExtension</t>
-  </si>
-  <si>
-    <t>List.identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Business identifier</t>
-  </si>
-  <si>
-    <t>Identifier for the List assigned for business purposes outside the context of FHIR.</t>
-  </si>
-  <si>
-    <t>.id</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>List.status</t>
-  </si>
-  <si>
-    <t>current | retired | entered-in-error</t>
-  </si>
-  <si>
-    <t>Indicates the current state of this list.</t>
-  </si>
-  <si>
-    <t>This element is labeled as a modifier because the status contains codes that mark the resource as not currently valid.</t>
-  </si>
-  <si>
-    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="current"/&gt;</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>The current state of the list</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/list-status</t>
-  </si>
-  <si>
-    <t>.status[current=active;retired=obsolete;entered-in-error=nullified]</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>List.mode</t>
-  </si>
-  <si>
-    <t>working | snapshot | changes</t>
-  </si>
-  <si>
-    <t>How this list was prepared - whether it is a working list that is suitable for being maintained on an ongoing basis, or if it represents a snapshot of a list of items from another source, or whether it is a prepared list where items may be marked as added, modified or deleted.</t>
-  </si>
-  <si>
-    <t>This element is labeled as a modifier because a change list must not be mis-understood as a complete list.</t>
-  </si>
-  <si>
-    <t>Lists are used in various ways, and it must be known in what way it is safe to use them.</t>
-  </si>
-  <si>
-    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="snapshot"/&gt;</t>
-  </si>
-  <si>
-    <t>The processing mode that applies to this list</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/list-mode</t>
-  </si>
-  <si>
-    <t>.outBoundRelationship[typeCode=COMP].target[classCode=OBS"].value</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>List.title</t>
   </si>
   <si>
     <t>Descriptive name for the list</t>
@@ -628,6 +496,9 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
+    <t>example</t>
+  </si>
+  <si>
     <t>What the purpose of a list is</t>
   </si>
   <si>
@@ -811,7 +682,22 @@
     <t>List.entry.id</t>
   </si>
   <si>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
     <t>List.entry.extension</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
   </si>
   <si>
     <t>changeDescription</t>
@@ -1096,7 +982,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL39"/>
+  <dimension ref="A1:AL32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1128,11 +1014,11 @@
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="95.21875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="40.30859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="49.78125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="34.0703125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1475,7 +1361,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s" s="2">
         <v>48</v>
@@ -1559,7 +1445,7 @@
         <v>41</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>41</v>
@@ -1570,7 +1456,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1587,21 +1473,23 @@
         <v>41</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="K5" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="K5" t="s" s="2">
+      <c r="L5" t="s" s="2">
         <v>63</v>
       </c>
-      <c r="L5" t="s" s="2">
+      <c r="M5" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
         <v>41</v>
@@ -1665,7 +1553,7 @@
         <v>41</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>41</v>
@@ -1673,18 +1561,18 @@
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>41</v>
@@ -1696,16 +1584,16 @@
         <v>41</v>
       </c>
       <c r="J6" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="K6" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="L6" t="s" s="2">
         <v>69</v>
       </c>
-      <c r="K6" t="s" s="2">
+      <c r="M6" t="s" s="2">
         <v>70</v>
-      </c>
-      <c r="L6" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M6" t="s" s="2">
-        <v>72</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -1731,37 +1619,37 @@
         <v>41</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="AB6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE6" t="s" s="2">
         <v>74</v>
       </c>
-      <c r="AC6" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD6" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE6" t="s" s="2">
-        <v>76</v>
-      </c>
       <c r="AF6" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>41</v>
@@ -1770,7 +1658,7 @@
         <v>41</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="AK6" t="s" s="2">
         <v>41</v>
@@ -1778,11 +1666,11 @@
     </row>
     <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
@@ -1798,10 +1686,10 @@
         <v>41</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s" s="2">
         <v>78</v>
@@ -1869,13 +1757,13 @@
         <v>48</v>
       </c>
       <c r="AH7" t="s" s="2">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="AI7" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ7" t="s" s="2">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="AK7" t="s" s="2">
         <v>41</v>
@@ -1883,18 +1771,18 @@
     </row>
     <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s" s="2">
         <v>41</v>
@@ -1903,19 +1791,19 @@
         <v>41</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -1965,13 +1853,13 @@
         <v>41</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG8" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH8" t="s" s="2">
         <v>41</v>
@@ -1980,7 +1868,7 @@
         <v>41</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="AK8" t="s" s="2">
         <v>41</v>
@@ -1988,7 +1876,7 @@
     </row>
     <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
@@ -1996,7 +1884,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s" s="2">
         <v>40</v>
@@ -2008,20 +1896,18 @@
         <v>41</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>92</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
         <v>41</v>
@@ -2058,19 +1944,17 @@
         <v>41</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB9" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>39</v>
@@ -2093,9 +1977,11 @@
     </row>
     <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>99</v>
+      </c>
       <c r="C10" t="s" s="2">
         <v>41</v>
       </c>
@@ -2104,7 +1990,7 @@
         <v>39</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>41</v>
@@ -2113,20 +1999,18 @@
         <v>41</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="M10" t="s" s="2">
-        <v>98</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>41</v>
@@ -2151,13 +2035,13 @@
         <v>41</v>
       </c>
       <c r="W10" t="s" s="2">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="X10" t="s" s="2">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="Y10" t="s" s="2">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="Z10" t="s" s="2">
         <v>41</v>
@@ -2175,7 +2059,7 @@
         <v>41</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>39</v>
@@ -2184,10 +2068,10 @@
         <v>40</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>41</v>
@@ -2198,11 +2082,11 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2215,22 +2099,22 @@
         <v>41</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
@@ -2256,13 +2140,13 @@
         <v>41</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>41</v>
@@ -2295,7 +2179,7 @@
         <v>41</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>41</v>
@@ -2314,29 +2198,27 @@
         <v>39</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>41</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="M12" t="s" s="2">
         <v>114</v>
       </c>
+      <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>41</v>
@@ -2385,30 +2267,30 @@
         <v>41</v>
       </c>
       <c r="AE12" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AF12" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG12" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH12" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI12" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ12" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="AF12" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG12" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH12" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI12" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ12" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="AK12" t="s" s="2">
-        <v>41</v>
+        <v>116</v>
       </c>
     </row>
-    <row r="13" hidden="true">
+    <row r="13">
       <c r="A13" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2416,22 +2298,22 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F13" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="K13" t="s" s="2">
         <v>118</v>
@@ -2448,7 +2330,7 @@
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" t="s" s="2">
-        <v>41</v>
+        <v>121</v>
       </c>
       <c r="R13" t="s" s="2">
         <v>41</v>
@@ -2466,13 +2348,13 @@
         <v>41</v>
       </c>
       <c r="W13" t="s" s="2">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>41</v>
@@ -2490,10 +2372,10 @@
         <v>41</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>48</v>
@@ -2505,23 +2387,23 @@
         <v>41</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>41</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>48</v>
@@ -2530,30 +2412,32 @@
         <v>41</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>126</v>
+        <v>67</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="N14" s="2"/>
+        <v>130</v>
+      </c>
+      <c r="N14" t="s" s="2">
+        <v>131</v>
+      </c>
       <c r="O14" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P14" s="2"/>
       <c r="Q14" t="s" s="2">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="R14" t="s" s="2">
         <v>41</v>
@@ -2571,13 +2455,13 @@
         <v>41</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>41</v>
@@ -2595,41 +2479,41 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>48</v>
       </c>
       <c r="AH14" t="s" s="2">
-        <v>131</v>
+        <v>41</v>
       </c>
       <c r="AI14" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>41</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>134</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>41</v>
@@ -2638,21 +2522,21 @@
         <v>41</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>137</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="N15" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="O15" t="s" s="2">
         <v>41</v>
       </c>
@@ -2664,7 +2548,7 @@
         <v>41</v>
       </c>
       <c r="S15" t="s" s="2">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="T15" t="s" s="2">
         <v>41</v>
@@ -2700,13 +2584,13 @@
         <v>41</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>41</v>
@@ -2715,15 +2599,15 @@
         <v>41</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2731,37 +2615,41 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="M16" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="N16" t="s" s="2">
+        <v>149</v>
+      </c>
       <c r="O16" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P16" s="2"/>
       <c r="Q16" t="s" s="2">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="R16" t="s" s="2">
         <v>41</v>
@@ -2779,26 +2667,28 @@
         <v>41</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB16" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="AB16" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="AC16" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
         <v>144</v>
@@ -2807,7 +2697,7 @@
         <v>39</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>41</v>
@@ -2816,49 +2706,51 @@
         <v>41</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>41</v>
+        <v>154</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>41</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>145</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
         <v>41</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>148</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="N17" t="s" s="2">
+        <v>161</v>
+      </c>
       <c r="O17" t="s" s="2">
         <v>41</v>
       </c>
@@ -2906,63 +2798,61 @@
         <v>41</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH17" t="s" s="2">
-        <v>149</v>
+        <v>41</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>41</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>41</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s" s="2">
         <v>41</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>72</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
         <v>41</v>
@@ -3011,13 +2901,13 @@
         <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>41</v>
@@ -3026,15 +2916,15 @@
         <v>41</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>41</v>
+        <v>169</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3045,28 +2935,32 @@
         <v>39</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="M19" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>175</v>
+      </c>
       <c r="O19" t="s" s="2">
         <v>41</v>
       </c>
@@ -3114,13 +3008,13 @@
         <v>41</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>41</v>
@@ -3129,23 +3023,23 @@
         <v>41</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>160</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>48</v>
@@ -3154,30 +3048,32 @@
         <v>49</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="N20" s="2"/>
+        <v>183</v>
+      </c>
+      <c r="N20" t="s" s="2">
+        <v>184</v>
+      </c>
       <c r="O20" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P20" s="2"/>
       <c r="Q20" t="s" s="2">
-        <v>165</v>
+        <v>41</v>
       </c>
       <c r="R20" t="s" s="2">
         <v>41</v>
@@ -3195,13 +3091,13 @@
         <v>41</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="X20" t="s" s="2">
-        <v>167</v>
+        <v>41</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>41</v>
@@ -3219,10 +3115,10 @@
         <v>41</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>48</v>
@@ -3234,15 +3130,15 @@
         <v>41</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3250,7 +3146,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>48</v>
@@ -3259,32 +3155,32 @@
         <v>41</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P21" s="2"/>
       <c r="Q21" t="s" s="2">
-        <v>176</v>
+        <v>41</v>
       </c>
       <c r="R21" t="s" s="2">
         <v>41</v>
@@ -3302,13 +3198,13 @@
         <v>41</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>41</v>
@@ -3326,10 +3222,10 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>48</v>
@@ -3341,15 +3237,15 @@
         <v>41</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>180</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3360,7 +3256,7 @@
         <v>39</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>41</v>
@@ -3369,21 +3265,19 @@
         <v>41</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>62</v>
+        <v>197</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="M22" s="2"/>
-      <c r="N22" t="s" s="2">
-        <v>184</v>
-      </c>
+      <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>41</v>
       </c>
@@ -3395,7 +3289,7 @@
         <v>41</v>
       </c>
       <c r="S22" t="s" s="2">
-        <v>185</v>
+        <v>41</v>
       </c>
       <c r="T22" t="s" s="2">
         <v>41</v>
@@ -3431,13 +3325,13 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>41</v>
@@ -3446,7 +3340,7 @@
         <v>41</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>41</v>
@@ -3454,7 +3348,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3465,7 +3359,7 @@
         <v>48</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>49</v>
@@ -3474,29 +3368,27 @@
         <v>41</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>192</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P23" s="2"/>
       <c r="Q23" t="s" s="2">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="R23" t="s" s="2">
         <v>41</v>
@@ -3514,13 +3406,13 @@
         <v>41</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>194</v>
+        <v>41</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>41</v>
@@ -3538,30 +3430,30 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>41</v>
+        <v>206</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>41</v>
+        <v>207</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>197</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3569,35 +3461,31 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F24" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>203</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>41</v>
       </c>
@@ -3645,7 +3533,7 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3660,15 +3548,15 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>205</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3679,7 +3567,7 @@
         <v>39</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>41</v>
@@ -3691,13 +3579,13 @@
         <v>41</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>207</v>
+        <v>93</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>208</v>
+        <v>94</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>209</v>
+        <v>95</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -3736,25 +3624,23 @@
         <v>41</v>
       </c>
       <c r="AA25" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB25" t="s" s="2">
-        <v>41</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="AB25" s="2"/>
       <c r="AC25" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD25" t="s" s="2">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH25" t="s" s="2">
         <v>41</v>
@@ -3763,17 +3649,19 @@
         <v>41</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>210</v>
+        <v>41</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>211</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="B26" t="s" s="2">
+        <v>216</v>
+      </c>
       <c r="C26" t="s" s="2">
         <v>41</v>
       </c>
@@ -3791,23 +3679,19 @@
         <v>41</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>217</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>41</v>
       </c>
@@ -3855,66 +3739,64 @@
         <v>41</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>41</v>
+        <v>103</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>41</v>
+        <v>220</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>218</v>
+        <v>41</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>219</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H27" t="s" s="2">
         <v>49</v>
-      </c>
-      <c r="H27" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>222</v>
+        <v>93</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="L27" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="L27" t="s" s="2">
-        <v>224</v>
-      </c>
       <c r="M27" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="N27" t="s" s="2">
-        <v>226</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
         <v>41</v>
       </c>
@@ -3962,13 +3844,13 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>41</v>
@@ -3977,15 +3859,15 @@
         <v>41</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>227</v>
+        <v>91</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>228</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3993,13 +3875,13 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>41</v>
@@ -4008,19 +3890,19 @@
         <v>41</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>41</v>
@@ -4045,13 +3927,11 @@
         <v>41</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="X28" t="s" s="2">
-        <v>235</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="X28" s="2"/>
       <c r="Y28" t="s" s="2">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>41</v>
@@ -4069,7 +3949,7 @@
         <v>41</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
@@ -4084,7 +3964,7 @@
         <v>41</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>237</v>
+        <v>135</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>41</v>
@@ -4092,7 +3972,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4103,30 +3983,34 @@
         <v>39</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+        <v>234</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>236</v>
+      </c>
       <c r="O29" t="s" s="2">
-        <v>41</v>
+        <v>237</v>
       </c>
       <c r="P29" s="2"/>
       <c r="Q29" t="s" s="2">
@@ -4172,30 +4056,30 @@
         <v>41</v>
       </c>
       <c r="AE29" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH29" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="AF29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="AI29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4203,13 +4087,13 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>41</v>
@@ -4218,18 +4102,20 @@
         <v>41</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="K30" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="N30" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="K30" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>41</v>
       </c>
@@ -4277,30 +4163,30 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>248</v>
+        <v>41</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>249</v>
+        <v>41</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="31" hidden="true">
+    <row r="31">
       <c r="A31" t="s" s="2">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4308,13 +4194,13 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F31" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>41</v>
@@ -4323,13 +4209,13 @@
         <v>41</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>62</v>
+        <v>247</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>63</v>
+        <v>248</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>64</v>
+        <v>249</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4380,10 +4266,10 @@
         <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>65</v>
+        <v>246</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>48</v>
@@ -4395,15 +4281,15 @@
         <v>41</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>66</v>
+        <v>250</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="32" hidden="true">
+    <row r="32">
       <c r="A32" t="s" s="2">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4414,10 +4300,10 @@
         <v>39</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>41</v>
@@ -4426,16 +4312,20 @@
         <v>41</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>143</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+        <v>253</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>255</v>
+      </c>
       <c r="O32" t="s" s="2">
         <v>41</v>
       </c>
@@ -4459,790 +4349,53 @@
         <v>41</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>41</v>
+        <v>192</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>41</v>
+        <v>256</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>41</v>
+        <v>257</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB32" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>41</v>
+      </c>
       <c r="AC32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD32" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>76</v>
+        <v>251</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>41</v>
+        <v>206</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>41</v>
+        <v>258</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="B33" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="C33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="H33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J33" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="K33" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P33" s="2"/>
-      <c r="Q33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" hidden="true">
-      <c r="A34" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H34" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="I34" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J34" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="K34" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="N34" s="2"/>
-      <c r="O34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P34" s="2"/>
-      <c r="Q34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE34" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F35" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G35" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="H35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J35" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="K35" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="O35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P35" s="2"/>
-      <c r="Q35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W35" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="X35" s="2"/>
-      <c r="Y35" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="Z35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="AF35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" hidden="true">
-      <c r="A36" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H36" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="I36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J36" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="K36" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="O36" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="P36" s="2"/>
-      <c r="Q36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE36" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="AF36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" hidden="true">
-      <c r="A37" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F37" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J37" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="K37" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P37" s="2"/>
-      <c r="Q37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE37" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AF37" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG37" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ37" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F38" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G38" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="H38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J38" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="K38" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P38" s="2"/>
-      <c r="Q38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE38" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="AF38" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="G39" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="H39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J39" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="K39" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="O39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P39" s="2"/>
-      <c r="Q39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W39" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="X39" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="Y39" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="Z39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE39" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="AF39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG39" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="AI39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="AK39" t="s" s="2">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK39">
+  <autoFilter ref="A1:AK32">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5252,7 +4405,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI38">
+  <conditionalFormatting sqref="A2:AI31">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>